<commit_message>
Updated Stand-up meeting for week-03
</commit_message>
<xml_diff>
--- a/Sprint3/Stand-up Meeting Sprint3.xlsx
+++ b/Sprint3/Stand-up Meeting Sprint3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Sprint3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A262EF72-943B-4158-AA78-BD2ADFF0F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA024423-7ABF-411A-820B-0C4F17B81E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -163,6 +163,24 @@
   <si>
     <t>We or on the process of database layouts and firebase database.</t>
   </si>
+  <si>
+    <t>Designed blueprint on login and logout pages and worked on layout pages.</t>
+  </si>
+  <si>
+    <t>will work on the backend code and created a blueprint to link the data entered by the user to the database.</t>
+  </si>
+  <si>
+    <t>Based on layout design I will write backend code to connect user entered data to database and Database to frontend.</t>
+  </si>
+  <si>
+    <t>If we notice any errors, we'll work to fix them.</t>
+  </si>
+  <si>
+    <t>If we encounter any error while connecting Database , we are going to fix those errors</t>
+  </si>
+  <si>
+    <t>I have designed ER diagrams in Lucid chart and drawn relationships between entities.</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -485,11 +503,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -546,6 +594,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,7 +819,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1152,7 +1206,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="9" t="s">
         <v>5</v>
@@ -1182,15 +1236,19 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1214,13 +1272,17 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14"/>
       <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1244,13 +1306,17 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15"/>
       <c r="B16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>31</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>

</xml_diff>